<commit_message>
added a tab for entering driven km and logic to process it in the .xlsxc file
</commit_message>
<xml_diff>
--- a/ExcelTemplates/StundenzettelTemplate.xlsx
+++ b/ExcelTemplates/StundenzettelTemplate.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Datum: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Beginn</t>
@@ -37,6 +40,18 @@
     <t>Arbeitsbeschreibung</t>
   </si>
   <si>
+    <t>Km Begin</t>
+  </si>
+  <si>
+    <t>Km Ende</t>
+  </si>
+  <si>
+    <t>Strecke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
     <t>Name:</t>
   </si>
   <si>
@@ -50,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -75,6 +90,11 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Lexend"/>
     </font>
     <font>
@@ -83,7 +103,7 @@
       <name val="Lexend"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +124,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFE6DD"/>
         <bgColor rgb="FFFFE6DD"/>
       </patternFill>
@@ -244,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -264,6 +290,9 @@
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -279,56 +308,68 @@
     <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="3" fontId="6" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="5" fontId="6" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="13" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -343,7 +384,15 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -618,33 +667,37 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="V10" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="C12" s="14" t="s">
+        <v>4</v>
+      </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="14" t="s">
-        <v>4</v>
+      <c r="E12" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="12" t="s">
+      <c r="I12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="J12" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -652,6 +705,15 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="5"/>
+      <c r="T12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="U12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="7"/>
@@ -671,517 +733,604 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="10"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="18"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="20"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="18"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="20"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="18"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="20"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="18"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="20"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="18"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="20"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="18"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="20"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="18"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="31"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="20"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="18"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="20"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="18"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="20"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="18"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="18"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="20"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="20"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="34"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="18"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="18"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="20"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="20"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="18"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="18"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="20"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="20"/>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+      <c r="V25" s="34"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="18"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="18"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="20"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="20"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="Y26" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="18"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="18"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="20"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="20"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="34"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="18"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="20"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="18"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="18"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="20"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="20"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="18"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="20"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="20"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="35"/>
+      <c r="V30" s="35"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="18"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="18"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="20"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="20"/>
+      <c r="T31" s="34"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="34"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="18"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="18"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="20"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="20"/>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
+      <c r="V32" s="35"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="18"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="18"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="20"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="20"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="18"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="18"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="20"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="20"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="18"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="18"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="20"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="20"/>
+      <c r="T35" s="34"/>
+      <c r="U35" s="34"/>
+      <c r="V35" s="34"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="18"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="18"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="20"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="35"/>
+      <c r="V36" s="35"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="18"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="18"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="20"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="20"/>
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="18"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="18"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="20"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="20"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
+      <c r="T39" s="40"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="41"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
+      <c r="T40" s="40"/>
+      <c r="U40" s="40"/>
+      <c r="V40" s="43"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="37" t="s">
-        <v>8</v>
+      <c r="A43" s="44" t="s">
+        <v>13</v>
       </c>
       <c r="B43" s="5"/>
-      <c r="C43" s="38"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="8"/>
@@ -1189,27 +1338,27 @@
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="37" t="s">
-        <v>9</v>
+      <c r="A45" s="44" t="s">
+        <v>14</v>
       </c>
       <c r="B45" s="5"/>
-      <c r="C45" s="38"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="40"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="40"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
+      <c r="A46" s="47"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="47"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="8"/>
@@ -2172,7 +2321,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="91">
+  <mergeCells count="95">
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="E37:G37"/>
@@ -2210,13 +2359,6 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="L12:R13"/>
-    <mergeCell ref="L15:R15"/>
-    <mergeCell ref="L16:R16"/>
-    <mergeCell ref="L17:R17"/>
-    <mergeCell ref="L14:R14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="E16:G16"/>
@@ -2264,6 +2406,17 @@
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="E27:G27"/>
+    <mergeCell ref="V39:V40"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="L12:R13"/>
+    <mergeCell ref="L15:R15"/>
+    <mergeCell ref="L16:R16"/>
+    <mergeCell ref="L17:R17"/>
+    <mergeCell ref="L14:R14"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added option to select a filepath for a signature image and made some other minor tweaks
</commit_message>
<xml_diff>
--- a/ExcelTemplates/StundenzettelTemplate.xlsx
+++ b/ExcelTemplates/StundenzettelTemplate.xlsx
@@ -16,7 +16,7 @@
     <t xml:space="preserve">Datum: </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>2023.12.24</t>
   </si>
   <si>
     <t>Beginn</t>
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -82,6 +82,12 @@
       <color theme="1"/>
       <name val="Lexend"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Lexend"/>
+    </font>
     <font/>
     <font>
       <sz val="18.0"/>
@@ -94,6 +100,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Lexend"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Lexend"/>
     </font>
@@ -124,14 +135,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
+        <fgColor rgb="FFFFE6DD"/>
+        <bgColor rgb="FFFFE6DD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE6DD"/>
-        <bgColor rgb="FFFFE6DD"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -270,129 +281,111 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="10" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="7" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="7" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="9" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="3" fontId="6" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="5" fontId="6" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="13" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
@@ -627,6 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -635,6 +629,7 @@
   <cols>
     <col customWidth="1" min="1" max="7" width="12.63"/>
     <col customWidth="1" min="8" max="8" width="2.63"/>
+    <col customWidth="1" min="9" max="10" width="12.63"/>
     <col customWidth="1" min="11" max="11" width="2.63"/>
   </cols>
   <sheetData>
@@ -648,55 +643,61 @@
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="V10" s="11" t="s">
-        <v>1</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="12" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="K12" s="14"/>
+      <c r="L12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="4"/>
@@ -705,13 +706,14 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="5"/>
-      <c r="T12" s="12" t="s">
+      <c r="S12" s="14"/>
+      <c r="T12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="U12" s="12" t="s">
+      <c r="U12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V12" s="12" t="s">
+      <c r="V12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -723,9 +725,10 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="7"/>
       <c r="J13" s="10"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="8"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -733,604 +736,688 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="10"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="20"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="20"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="31"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="20"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="20"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="20"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="20"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="31"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="20"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="20"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="20"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="20"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="20"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="34"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="31"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="20"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="20"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="20"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="34"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="31"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="20"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="20"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
-      <c r="Y26" s="11" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="Y26" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="20"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="34"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="20"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="20"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="20"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="20"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="34"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="35"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="20"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="20"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="20"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="20"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="34"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="31"/>
+      <c r="V31" s="31"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="20"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="20"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="20"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="20"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="34"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="31"/>
+      <c r="U33" s="31"/>
+      <c r="V33" s="31"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="35"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="20"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="20"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="20"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="20"/>
-      <c r="T35" s="34"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="34"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="35"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="20"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="20"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="20"/>
-      <c r="T37" s="34"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="34"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="20"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="20"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="35"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="39"/>
-      <c r="T39" s="40"/>
-      <c r="U39" s="40"/>
-      <c r="V39" s="41"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="34"/>
+      <c r="U39" s="34"/>
+      <c r="V39" s="35"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="42"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
-      <c r="T40" s="40"/>
-      <c r="U40" s="40"/>
-      <c r="V40" s="43"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="34"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="7"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="42"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="42"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="5"/>
-      <c r="C43" s="45"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="8"/>
@@ -1338,27 +1425,27 @@
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="5"/>
-      <c r="C45" s="45"/>
+      <c r="C45" s="40"/>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="47"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="47"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="41"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="8"/>
@@ -2322,102 +2409,105 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="C43:E44"/>
-    <mergeCell ref="C45:E47"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="A45:B47"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="L23:R23"/>
+    <mergeCell ref="L24:R24"/>
+    <mergeCell ref="L16:R16"/>
+    <mergeCell ref="L17:R17"/>
     <mergeCell ref="L18:R18"/>
     <mergeCell ref="L19:R19"/>
     <mergeCell ref="L20:R20"/>
     <mergeCell ref="L21:R21"/>
     <mergeCell ref="L22:R22"/>
-    <mergeCell ref="L23:R23"/>
-    <mergeCell ref="L24:R24"/>
-    <mergeCell ref="L32:R32"/>
-    <mergeCell ref="L34:R34"/>
-    <mergeCell ref="L35:R35"/>
-    <mergeCell ref="L36:R36"/>
-    <mergeCell ref="L37:R37"/>
-    <mergeCell ref="L38:R38"/>
-    <mergeCell ref="L33:R33"/>
-    <mergeCell ref="L25:R25"/>
     <mergeCell ref="L26:R26"/>
     <mergeCell ref="L27:R27"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="L25:R25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
     <mergeCell ref="L28:R28"/>
     <mergeCell ref="L29:R29"/>
     <mergeCell ref="L30:R30"/>
     <mergeCell ref="L31:R31"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="L34:R34"/>
+    <mergeCell ref="L35:R35"/>
+    <mergeCell ref="L36:R36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="V39:V40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="L37:R37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="L38:R38"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="L12:R13"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="L14:R14"/>
+    <mergeCell ref="A1:F7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D10"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:D13"/>
     <mergeCell ref="E12:G13"/>
-    <mergeCell ref="A1:F6"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="L15:R15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="V39:V40"/>
-    <mergeCell ref="T12:T13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="L12:R13"/>
-    <mergeCell ref="L15:R15"/>
-    <mergeCell ref="L16:R16"/>
-    <mergeCell ref="L17:R17"/>
-    <mergeCell ref="L14:R14"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:E44"/>
+    <mergeCell ref="A45:B47"/>
+    <mergeCell ref="C45:E47"/>
   </mergeCells>
+  <printOptions/>
+  <pageMargins bottom="0.5" footer="0.0" header="0.0" left="0.75" right="0.75" top="0.75"/>
+  <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>